<commit_message>
python notebook with bag of words and word2vec
</commit_message>
<xml_diff>
--- a/mini/WHO_FAQ.xlsx
+++ b/mini/WHO_FAQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma 1/Documents/Triple/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghn\Documents\GitHub\NLP_AutomaticGradingSystem\mini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833A93AA-EE15-B642-99AD-BC0B045C3D73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A5FF84-7414-48B8-B88F-A3AF626DB247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2000" windowWidth="27840" windowHeight="17060" xr2:uid="{C9DB26B1-B960-944C-B948-2AA9B2AD07F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9DB26B1-B960-944C-B948-2AA9B2AD07F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Context</t>
   </si>
@@ -45,9 +39,6 @@
     <t>Coronaviruses are a large family of viruses which may cause illness in animals or humans. </t>
   </si>
   <si>
-    <t>In humans, several coronaviruses are known to cause respiratory infections ranging from the common cold to more severe diseases</t>
-  </si>
-  <si>
     <t>What is COVID-19?</t>
   </si>
   <si>
@@ -60,24 +51,12 @@
     <t>The most common symptoms of COVID-19 are fever, tiredness, and dry cough. Some patients may have aches and pains, nasal congestion, runny nose, sore throat or diarrhea. These symptoms are usually mild and begin gradually.</t>
   </si>
   <si>
-    <t>Some people become infected but don’t develop any symptoms and don't feel unwell. Most people (about 80%) recover from the disease without needing special treatment.</t>
-  </si>
-  <si>
-    <t>Around 1 out of every 6 people who gets COVID-19 becomes seriously ill and develops difficulty breathing. </t>
-  </si>
-  <si>
-    <t>Older people, and those with underlying medical problems like high blood pressure, heart problems or diabetes, are more likely to develop serious illness. People with fever, cough and difficulty breathing should seek medical attention.</t>
-  </si>
-  <si>
     <t>How does COVID-19 spread?</t>
   </si>
   <si>
     <t>People can catch COVID-19 from others who have the virus. The disease can spread from person to person through small droplets from the nose or mouth which are spread when a person with COVID-19 coughs or exhales. </t>
   </si>
   <si>
-    <t>People can also catch COVID-19 if they breathe in droplets from a person with COVID-19 who coughs out or exhales droplets. This is why it is important to stay more than 1 meter (3 feet) away from a person who is sick.</t>
-  </si>
-  <si>
     <t>Can the virus that causes COVID-19 be transmitted through the air?</t>
   </si>
   <si>
@@ -90,39 +69,12 @@
     <t>The main way the disease spreads is through respiratory droplets expelled by someone who is coughing. The risk of catching COVID-19 from someone with no symptoms at all is very low.</t>
   </si>
   <si>
-    <t xml:space="preserve">Many people with COVID-19 experience only mild symptoms. This is particularly true at the early stages of the disease. It is therefore possible to catch COVID-19 from someone who has, for example, just a mild cough and does not feel ill. </t>
-  </si>
-  <si>
     <t>Can I catch COVID-19 from the feces of someone with the disease?</t>
   </si>
   <si>
     <t xml:space="preserve">The risk of catching COVID-19 from the feces of an infected person appears to be low. While initial investigations suggest the virus may be present in feces in some cases, spread through this route is not a main feature of the outbreak. </t>
   </si>
   <si>
-    <t>What can I do to protect myself and prevent the spread of disease?</t>
-  </si>
-  <si>
-    <t>Regularly and thoroughly clean your hands with an alcohol-based hand rub or wash them with soap and water.</t>
-  </si>
-  <si>
-    <t>Maintain at least 1 metre (3 feet) distance between yourself and anyone who is coughing or sneezing.</t>
-  </si>
-  <si>
-    <t>Avoid touching eyes, nose and mouth.</t>
-  </si>
-  <si>
-    <t>Make sure you, and the people around you, follow good respiratory hygiene. This means covering your mouth and nose with your bent elbow or tissue when you cough or sneeze. Then dispose of the used tissue immediately.</t>
-  </si>
-  <si>
-    <t>Stay home if you feel unwell. If you have a fever, cough and difficulty breathing, seek medical attention and call in advance. Follow the directions of your local health authority.</t>
-  </si>
-  <si>
-    <t>Keep up to date on the latest COVID-19 hotspots (cities or local areas where COVID-19 is spreading widely).</t>
-  </si>
-  <si>
-    <t>If possible, avoid traveling to places  – especially if you are an older person or have diabetes, heart or lung disease.</t>
-  </si>
-  <si>
     <t>What can I do to protect myself andProtection measures for persons who are in or have recently visited (past 14 days) areas where COVID-19 is spreading prevent the spread of disease?</t>
   </si>
   <si>
@@ -141,9 +93,6 @@
     <t>The risk depends on where you  are - and more specifically, whether there is a COVID-19 outbreak unfolding there.</t>
   </si>
   <si>
-    <t>For most people in most locations the risk of catching COVID-19 is still low. However, there are now places around the world (cities or areas) where the disease is spreading. For people living in, or visiting, these areas the risk of catching COVID-19 is higher.</t>
-  </si>
-  <si>
     <t>COVID-19 outbreaks can be contained and transmission stopped, as has been shown in China and some other countries. Unfortunately, new outbreaks can emerge rapidly. It’s important to be aware of the situation where you are or intend to go.</t>
   </si>
   <si>
@@ -153,9 +102,6 @@
     <t>Illness due to COVID-19 infection is generally mild, especially for children and young adults. However, it can cause serious illness: about 1 in every 5 people who catch it need hospital care.</t>
   </si>
   <si>
-    <t>We can channel our concerns into actions to protect ourselves, our loved ones and our communities.</t>
-  </si>
-  <si>
     <t>Who is at risk of developing severe illness?</t>
   </si>
   <si>
@@ -168,111 +114,60 @@
     <t>No. Antibiotics do not work against viruses, they only work on bacterial infections. COVID-19 is caused by a virus, so antibiotics do not work. </t>
   </si>
   <si>
-    <t>Antibiotics should not be used as a means of prevention or treatment of COVID-19. They should only be used as directed by a physician to treat a bacterial infection. </t>
-  </si>
-  <si>
     <t>Are there any medicines or therapies that can prevent or cure COVID-19?</t>
   </si>
   <si>
     <t>While some western, traditional or home remedies may provide comfort and alleviate symptoms of COVID-19, there is no evidence that current medicine can prevent or cure the disease. </t>
   </si>
   <si>
-    <t>WHO does not recommend self-medication with any medicines, including antibiotics, as a prevention or cure for COVID-19.</t>
-  </si>
-  <si>
     <t>Is there a vaccine, drug or treatment for COVID-19?</t>
   </si>
   <si>
     <t>Not yet. To date, there is no vaccine and no specific antiviral medicine to prevent or treat COVID-2019. </t>
   </si>
   <si>
-    <t>Those affected should receive care to relieve symptoms. People with serious illness should be hospitalized. Most patients recover thanks to supportive care.</t>
-  </si>
-  <si>
-    <t>Possible vaccines and some specific drug treatments are under investigation. They are being tested through clinical trials. WHO is coordinating efforts to develop vaccines and medicines to prevent and treat COVID-19.</t>
-  </si>
-  <si>
-    <t>The most effective ways to protect yourself and others against COVID-19 are to frequently clean your hands, cover your cough with the bend of elbow or tissue, and maintain a distance of at least 1 meter (3 feet) from people who are coughing or sneezing.</t>
-  </si>
-  <si>
     <t>Is COVID-19 the same as SARS?</t>
   </si>
   <si>
     <t>No. The virus that causes COVID-19 and the one that caused the outbreak of Severe Acute Respiratory Syndrome (SARS) in 2003 are related to each other genetically, but the diseases they cause are quite different.</t>
   </si>
   <si>
-    <t>SARS was more deadly but much less infectious than COVID-19. There have been no outbreaks of SARS anywhere in the world since 2003.</t>
-  </si>
-  <si>
     <t>Should I wear a mask to protect myself</t>
   </si>
   <si>
     <t>Only wear a mask if you are ill with COVID-19 symptoms (especially coughing) or looking after someone who may have COVID-19. Disposable face mask can only be used once.</t>
   </si>
   <si>
-    <t>If you are not ill or looking after someone who is ill then you are wasting a mask. </t>
-  </si>
-  <si>
-    <t>There is a world-wide shortage of masks, so WHO urges people to use masks wisely.</t>
-  </si>
-  <si>
     <t>How to put on, use, take off and dispose of a mask?</t>
   </si>
   <si>
     <t>Remember, a mask should only be used by health workers, care takers, and individuals with respiratory symptoms, such as fever and cough.</t>
   </si>
   <si>
-    <t>Before touching the mask, clean hands with an alcohol-based hand rub or soap and water</t>
-  </si>
-  <si>
     <t>How long is the incubation period for COVID-19?</t>
   </si>
   <si>
     <t>The “incubation period” means the time between catching the virus and beginning to have symptoms of the disease.</t>
   </si>
   <si>
-    <t>Most estimates of the incubation period for COVID-19 range from 1-14 days, most commonly around five days. These estimates will be updated as more data become available.</t>
-  </si>
-  <si>
     <t>Can humans be infected with the COVID-19 from an animal source?</t>
   </si>
   <si>
     <t>Coronaviruses are a large family of viruses that are common in animals. Occasionally, people get infected with these viruses which may then spread to other people.</t>
   </si>
   <si>
-    <t xml:space="preserve">SARS-CoV was associated with civet cats and MERS-CoV is transmitted by dromedary camels. </t>
-  </si>
-  <si>
-    <t>Possible animal sources of COVID-19 have not yet been confirmed.  </t>
-  </si>
-  <si>
-    <t>To protect yourself, such as when visiting live animal markets, avoid direct contact with animals and surfaces in contact with animals.</t>
-  </si>
-  <si>
-    <t>Handle raw meat, milk or animal organs with care to avoid contamination of uncooked foods and avoid consuming raw or undercooked animal products.</t>
-  </si>
-  <si>
     <t>Can I catch COVID-19 from my pet?</t>
   </si>
   <si>
     <t>While there has been one instance of a dog being infected in Hong Kong, to date, there is no evidence that a dog, cat or any pet can transmit COVID-19.</t>
   </si>
   <si>
-    <t>COVID-19 is mainly spread through droplets produced when an infected person coughs, sneezes, or speaks.</t>
-  </si>
-  <si>
     <t>How long does the virus survive on surfaces?</t>
   </si>
   <si>
     <t>It is not certain how long the virus that causes COVID-19 survives on surfaces, but it seems to behave like other coronaviruses.</t>
   </si>
   <si>
-    <t>Studies suggest that coronaviruses (including preliminary information on the COVID-19 virus) may persist on surfaces for a few hours or up to several days. This may vary under different conditions (e.g. type of surface, temperature or humidity of the environment).</t>
-  </si>
-  <si>
-    <t>If you think a surface may be infected, clean it with simple disinfectant to kill the virus and protect yourself and others.</t>
-  </si>
-  <si>
     <t>Is it safe to receive a package from any area where COVID-19 has been reported?</t>
   </si>
   <si>
@@ -282,15 +177,9 @@
     <t>Is there anything I should not do?</t>
   </si>
   <si>
-    <t>Smoking</t>
-  </si>
-  <si>
     <t>Wearing multiple masks</t>
   </si>
   <si>
-    <t>Taking antibiotics</t>
-  </si>
-  <si>
     <t>Is the source causing COVID-19 known?</t>
   </si>
   <si>
@@ -303,12 +192,6 @@
     <t>The first human cases of COVID-19 were identified in Wuhan City, China in December 2019.</t>
   </si>
   <si>
-    <t>SARS-CoV, the virus which caused the SARS outbreak in 2003, jumped from an animal reservoir (civet cats, a farmed wild animal) to humans and then spread between humans. </t>
-  </si>
-  <si>
-    <t>Until the source of this virus is identified and controlled, there is a risk of reintroduction of the virus in the human population and the risk of new outbreaks like the ones we are currently experiencing.</t>
-  </si>
-  <si>
     <t>Is COVID-19 airborne?</t>
   </si>
   <si>
@@ -321,18 +204,12 @@
     <t>At present there is no evidence that they are at higher risk of severe illness than the general population.</t>
   </si>
   <si>
-    <t>due to changes in their bodies and immune systems, we know that pregnant women can be badly affected by some respiratory infections. It is therefore important that they take precautions to protect themselves against COVID-19, and report possible symptoms (including fever, cough or difficulty breathing) to their healthcare provider.</t>
-  </si>
-  <si>
     <t>I'm pregnant. How can I protect myself against COVID-19?</t>
   </si>
   <si>
     <t>Pregnant women should take the same precautions to avoid COVID-19 infection as other people.</t>
   </si>
   <si>
-    <t>Pregnant women and women who have recently delivered – including those affected by COVID-19 - should attend their routine care appointments. </t>
-  </si>
-  <si>
     <t>Should pregnant women be tested for COVID-19?</t>
   </si>
   <si>
@@ -375,21 +252,12 @@
     <t>COVID-19 and influenza viruses have a similar disease presentation. That is, they both cause respiratory disease, which presents as a wide range of illness from asymptomatic or mild through to severe disease and death.</t>
   </si>
   <si>
-    <t>Both viruses are transmitted by contact, droplets and fomites.</t>
-  </si>
-  <si>
     <t>How are COVID-19 and influenza viruses different?</t>
   </si>
   <si>
     <t>The speed of transmission is an important point of difference between the two viruses. Influenza has a shorter median incubation period (the time from infection to appearance of symptoms) and a shorter serial interval (the time between successive cases) than COVID-19 virus.</t>
   </si>
   <si>
-    <t>Those most at risk for severe influenza infection are children, pregnant women, elderly, those with underlying chronic medical conditions and those who are immunosuppressed.</t>
-  </si>
-  <si>
-    <t>Mortality for COVID-19 appears higher than for influenza, especially seasonal influenza.</t>
-  </si>
-  <si>
     <t>What medical interventions are available for COVID-19 and influenza viruses?</t>
   </si>
   <si>
@@ -399,9 +267,6 @@
     <t>Are smokers and tobacco users at higher risk of COVID-19 infection?</t>
   </si>
   <si>
-    <t>Smokers are likely to be more vulnerable to COVID-19 as the act of smoking means that fingers (and possibly contaminated cigarettes) are in contact with lips which increases the possibility of transmission of virus from hand to mouth.</t>
-  </si>
-  <si>
     <t>Smoking products such as water pipes often involve the sharing of mouth pieces and hoses, which could facilitate the transmission of COVID-19 in communal and social settings.</t>
   </si>
   <si>
@@ -409,9 +274,6 @@
   </si>
   <si>
     <t>High profile international sporting events such as the Olympics or World Cups as well as international religious events such as the Hajj count as mass gatherings.</t>
-  </si>
-  <si>
-    <t>An event counts as a “mass gatherings” if the number of people it brings together is so large that it has the potential to strain the planning and response resources of the health system in the community where it takes place. </t>
   </si>
   <si>
     <t>Does WHO recommend that all international mass gatherings be cancelled because of COVID-19?</t>
@@ -493,19 +355,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -521,7 +382,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -817,13 +678,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6678A23-C73C-894C-B40D-72507169EEC1}">
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+      <selection activeCell="A70" activeCellId="27" sqref="A16:XFD16 A18:XFD18 A20:XFD20 A21:XFD21 A22:XFD22 A24:XFD24 A26:XFD26 A27:XFD27 A29:XFD29 A31:XFD31 A33:XFD33 A35:XFD35 A34:XFD34 A36:XFD36 A38:XFD38 A40:XFD40 A41:XFD41 A43:XFD43 A45:XFD45 A48:XFD48 A49:XFD49 A52:XFD52 A54:XFD54 A64:XFD64 A65:XFD65 A62:XFD62 A67:XFD67 A70:XFD70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
     <col min="2" max="2" width="75.33203125" customWidth="1"/>
@@ -849,879 +710,490 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
+      <c r="A6" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
+      <c r="A10" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
+      <c r="A17" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
+      <c r="A18" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
+      <c r="A20" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
+      <c r="A21" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
+      <c r="A22" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4" t="s">
-        <v>31</v>
+      <c r="A23" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4" t="s">
-        <v>34</v>
+      <c r="A24" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4" t="s">
-        <v>34</v>
+      <c r="A25" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4" t="s">
-        <v>34</v>
+      <c r="A26" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>39</v>
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>71</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>55</v>
+        <v>73</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>59</v>
+      <c r="A41" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>60</v>
+      <c r="A42" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>62</v>
+      <c r="A43" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="A45" s="6"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
       <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="2"/>
+      <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="2"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="2"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="2"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="2"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="2"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C59" s="2"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="2"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C61" s="2"/>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="2"/>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C63" s="2"/>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C71" s="2"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C86" s="2"/>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="7"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A82" r:id="rId1" display="https://www.who.int/news-room/q-a-detail/q-a-on-smoking-and-covid-19" xr:uid="{D84E903A-01FC-E44C-970A-ACA64C7B7BFB}"/>
-    <hyperlink ref="A83" r:id="rId2" display="https://www.who.int/news-room/q-a-detail/q-a-on-smoking-and-covid-19" xr:uid="{3EA477C8-FEFD-9245-AD67-709E02EFBFA9}"/>
-    <hyperlink ref="A84" r:id="rId3" display="https://www.who.int/news-room/q-a-detail/q-a-on-mass-gatherings-and-covid-19" xr:uid="{DBA79294-4C32-0746-BAC5-D8FFF1296601}"/>
-    <hyperlink ref="A85" r:id="rId4" display="https://www.who.int/news-room/q-a-detail/q-a-on-mass-gatherings-and-covid-19" xr:uid="{AEEDE984-8055-0548-8003-4BACA4FB6DA7}"/>
-    <hyperlink ref="A86" r:id="rId5" display="https://www.who.int/news-room/q-a-detail/q-a-on-mass-gatherings-and-covid-19" xr:uid="{30CFBE30-FD73-D64D-AC8F-5F86170F8F32}"/>
+    <hyperlink ref="A41" r:id="rId1" display="https://www.who.int/news-room/q-a-detail/q-a-on-smoking-and-covid-19" xr:uid="{3EA477C8-FEFD-9245-AD67-709E02EFBFA9}"/>
+    <hyperlink ref="A42" r:id="rId2" display="https://www.who.int/news-room/q-a-detail/q-a-on-mass-gatherings-and-covid-19" xr:uid="{DBA79294-4C32-0746-BAC5-D8FFF1296601}"/>
+    <hyperlink ref="A43" r:id="rId3" display="https://www.who.int/news-room/q-a-detail/q-a-on-mass-gatherings-and-covid-19" xr:uid="{30CFBE30-FD73-D64D-AC8F-5F86170F8F32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>